<commit_message>
report prepared for CIP 4, only task d missing
</commit_message>
<xml_diff>
--- a/CIP_4/CIP_04_DoWES.Parameters_Tower_modal_analysis.SS2016.00.xlsx
+++ b/CIP_4/CIP_04_DoWES.Parameters_Tower_modal_analysis.SS2016.00.xlsx
@@ -11,23 +11,23 @@
     <sheet name="Tower_design" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="alpha_A1_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$24</definedName>
-    <definedName function="false" hidden="false" name="alpha_A2_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$25</definedName>
-    <definedName function="false" hidden="false" name="alpha_A3_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$26</definedName>
-    <definedName function="false" hidden="false" name="cp_Betz" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$D$34</definedName>
-    <definedName function="false" hidden="false" name="c_l1_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$18</definedName>
-    <definedName function="false" hidden="false" name="c_l2_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$19</definedName>
-    <definedName function="false" hidden="false" name="c_l3_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$20</definedName>
-    <definedName function="false" hidden="false" name="diameter_br" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$I$41</definedName>
-    <definedName function="false" hidden="false" name="d_tower_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']Turm!$C$7</definedName>
-    <definedName function="false" hidden="false" name="E_steel" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$D$32</definedName>
-    <definedName function="false" hidden="false" name="f0_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']Turm!$C$6</definedName>
-    <definedName function="false" hidden="false" name="hh_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$16</definedName>
-    <definedName function="false" hidden="false" name="lambda_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$13</definedName>
-    <definedName function="false" hidden="false" name="length_blade_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$10</definedName>
-    <definedName function="false" hidden="false" name="length_br_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$17</definedName>
-    <definedName function="false" hidden="false" name="mass_nac_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']Turm!$C$3</definedName>
-    <definedName function="false" hidden="false" name="mass_rotor_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']Turm!$C$4</definedName>
+    <definedName function="false" hidden="false" name="alpha_A1_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$24</definedName>
+    <definedName function="false" hidden="false" name="alpha_A2_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$25</definedName>
+    <definedName function="false" hidden="false" name="alpha_A3_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$26</definedName>
+    <definedName function="false" hidden="false" name="cp_Betz" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$d$34</definedName>
+    <definedName function="false" hidden="false" name="c_l1_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$18</definedName>
+    <definedName function="false" hidden="false" name="c_l2_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$19</definedName>
+    <definedName function="false" hidden="false" name="c_l3_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$20</definedName>
+    <definedName function="false" hidden="false" name="diameter_br" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$i$41</definedName>
+    <definedName function="false" hidden="false" name="d_tower_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']turm!$c$7</definedName>
+    <definedName function="false" hidden="false" name="E_steel" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$d$32</definedName>
+    <definedName function="false" hidden="false" name="f0_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']turm!$c$6</definedName>
+    <definedName function="false" hidden="false" name="hh_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$16</definedName>
+    <definedName function="false" hidden="false" name="lambda_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$13</definedName>
+    <definedName function="false" hidden="false" name="length_blade_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$10</definedName>
+    <definedName function="false" hidden="false" name="length_br_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$17</definedName>
+    <definedName function="false" hidden="false" name="mass_nac_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']turm!$c$3</definedName>
+    <definedName function="false" hidden="false" name="mass_rotor_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']turm!$c$4</definedName>
     <definedName function="false" hidden="false" name="mass_s10_ref" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" name="mass_s1_ref" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" name="mass_s2_ref" vbProcedure="false">#ref!</definedName>
@@ -38,18 +38,18 @@
     <definedName function="false" hidden="false" name="mass_s7_ref" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" name="mass_s8_ref" vbProcedure="false">#ref!</definedName>
     <definedName function="false" hidden="false" name="mass_s9_ref" vbProcedure="false">#ref!</definedName>
-    <definedName function="false" hidden="false" name="nr_blades_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$15</definedName>
-    <definedName function="false" hidden="false" name="p_Betz_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$O$59</definedName>
-    <definedName function="false" hidden="false" name="p_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$4</definedName>
-    <definedName function="false" hidden="false" name="rho_air" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$D$30</definedName>
-    <definedName function="false" hidden="false" name="rho_steel" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$D$31</definedName>
-    <definedName function="false" hidden="false" name="R_prec_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$9</definedName>
-    <definedName function="false" hidden="false" name="R_round_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$11</definedName>
+    <definedName function="false" hidden="false" name="nr_blades_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$15</definedName>
+    <definedName function="false" hidden="false" name="p_Betz_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$o$59</definedName>
+    <definedName function="false" hidden="false" name="p_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$4</definedName>
+    <definedName function="false" hidden="false" name="rho_air" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$d$30</definedName>
+    <definedName function="false" hidden="false" name="rho_steel" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$d$31</definedName>
+    <definedName function="false" hidden="false" name="R_prec_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$9</definedName>
+    <definedName function="false" hidden="false" name="R_round_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$11</definedName>
     <definedName function="false" hidden="false" name="R_round_ref" vbProcedure="false">#ref!</definedName>
-    <definedName function="false" hidden="false" name="thick_tower_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']Turm!$C$10</definedName>
-    <definedName function="false" hidden="false" name="vrot_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$8</definedName>
-    <definedName function="false" hidden="false" name="vr_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$7</definedName>
-    <definedName function="false" hidden="false" name="vtipmax_red" vbProcedure="false">['file:///home/jjtl/working/Lehre/Design_of_wind_energy_systems/2016/CIP_Tutorial_04_-_Tower_design/Lehre/Aeroelastic Simulation of Wind Turbines/2012/Solutions/Tutorial 1 - Rotor Design and BEM advanced I - start_values.03.solutions.xlsx']'BEM easy'!$C$14</definedName>
+    <definedName function="false" hidden="false" name="thick_tower_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']turm!$c$10</definedName>
+    <definedName function="false" hidden="false" name="vrot_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$8</definedName>
+    <definedName function="false" hidden="false" name="vr_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$7</definedName>
+    <definedName function="false" hidden="false" name="vtipmax_red" vbProcedure="false">['file:///home/jjtl/working/lehre/design_of_wind_energy_systems/2016/cip_tutorial_04_-_tower_design/lehre/aeroelastic simulation of wind turbines/2012/solutions/tutorial 1 - rotor design and bem advanced i - start_values.03.solutions.xlsx']'bem easy'!$c$14</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -91,7 +91,7 @@
     <t>Grey</t>
   </si>
   <si>
-    <t>Electrical power </t>
+    <t>Electrical power</t>
   </si>
   <si>
     <t>kW</t>
@@ -109,7 +109,7 @@
     <t>kg</t>
   </si>
   <si>
-    <t>Rotor mass </t>
+    <t>Rotor mass</t>
   </si>
   <si>
     <t>Rotor speed</t>
@@ -149,10 +149,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -248,50 +250,50 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF008080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCC1DA"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBEEF4"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
         <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF33CCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCC1DA"/>
-        <bgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDBEEF4"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
@@ -387,15 +389,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -404,6 +402,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -428,11 +430,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -480,11 +478,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="10" fillId="15" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="14" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="15" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="10" fillId="15" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="10" fillId="15" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -496,8 +502,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Neutral" xfId="21" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -567,265 +573,256 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C1:N18"/>
+  <dimension ref="C1:N27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.1428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="46.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5714285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="5" style="1" width="12.1377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="11.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.2914979757085"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5668016194332"/>
+    <col collapsed="false" hidden="false" max="14" min="5" style="0" width="12.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.417004048583"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
-      <c r="L1" s="0"/>
-      <c r="M1" s="0"/>
-      <c r="N1" s="0"/>
-    </row>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="14" t="s">
+    <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="16" t="n">
+      <c r="E3" s="15" t="n">
         <v>1500</v>
       </c>
-      <c r="F3" s="16" t="n">
+      <c r="F3" s="15" t="n">
         <v>1500</v>
       </c>
-      <c r="G3" s="16" t="n">
+      <c r="G3" s="15" t="n">
         <v>1500</v>
       </c>
-      <c r="H3" s="16" t="n">
+      <c r="H3" s="15" t="n">
         <v>2500</v>
       </c>
-      <c r="I3" s="16" t="n">
+      <c r="I3" s="15" t="n">
         <v>2500</v>
       </c>
-      <c r="J3" s="16" t="n">
+      <c r="J3" s="15" t="n">
         <v>2500</v>
       </c>
-      <c r="K3" s="16" t="n">
+      <c r="K3" s="15" t="n">
         <v>3500</v>
       </c>
-      <c r="L3" s="16" t="n">
+      <c r="L3" s="15" t="n">
         <v>3500</v>
       </c>
-      <c r="M3" s="16" t="n">
+      <c r="M3" s="15" t="n">
         <v>3500</v>
       </c>
-      <c r="N3" s="16" t="n">
+      <c r="N3" s="15" t="n">
         <v>5000</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="14" t="s">
+    <row r="4" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="17" t="n">
+      <c r="E4" s="16" t="n">
         <v>80</v>
       </c>
-      <c r="F4" s="17" t="n">
+      <c r="F4" s="16" t="n">
         <v>85</v>
       </c>
-      <c r="G4" s="17" t="n">
+      <c r="G4" s="16" t="n">
         <v>100</v>
       </c>
-      <c r="H4" s="17" t="n">
+      <c r="H4" s="16" t="n">
         <v>85</v>
       </c>
-      <c r="I4" s="17" t="n">
+      <c r="I4" s="16" t="n">
         <v>100</v>
       </c>
-      <c r="J4" s="17" t="n">
+      <c r="J4" s="16" t="n">
         <v>115</v>
       </c>
-      <c r="K4" s="17" t="n">
+      <c r="K4" s="16" t="n">
         <v>100</v>
       </c>
-      <c r="L4" s="17" t="n">
+      <c r="L4" s="16" t="n">
         <v>115</v>
       </c>
-      <c r="M4" s="17" t="n">
+      <c r="M4" s="16" t="n">
         <v>130</v>
       </c>
-      <c r="N4" s="17" t="n">
+      <c r="N4" s="16" t="n">
         <v>140</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="18" t="s">
+    <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="17" t="n">
+      <c r="E5" s="16" t="n">
         <v>140000</v>
       </c>
-      <c r="F5" s="17" t="n">
+      <c r="F5" s="16" t="n">
         <v>140000</v>
       </c>
-      <c r="G5" s="17" t="n">
+      <c r="G5" s="16" t="n">
         <v>140000</v>
       </c>
-      <c r="H5" s="17" t="n">
+      <c r="H5" s="16" t="n">
         <v>200000</v>
       </c>
-      <c r="I5" s="17" t="n">
+      <c r="I5" s="16" t="n">
         <v>200000</v>
       </c>
-      <c r="J5" s="17" t="n">
+      <c r="J5" s="16" t="n">
         <v>200000</v>
       </c>
-      <c r="K5" s="17" t="n">
+      <c r="K5" s="16" t="n">
         <v>260000</v>
       </c>
-      <c r="L5" s="17" t="n">
+      <c r="L5" s="16" t="n">
         <v>260000</v>
       </c>
-      <c r="M5" s="17" t="n">
+      <c r="M5" s="16" t="n">
         <v>260000</v>
       </c>
-      <c r="N5" s="17" t="n">
+      <c r="N5" s="16" t="n">
         <v>320000</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="18" t="s">
+    <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="17" t="n">
+      <c r="E6" s="16" t="n">
         <v>45000</v>
       </c>
-      <c r="F6" s="17" t="n">
+      <c r="F6" s="16" t="n">
         <v>45000</v>
       </c>
-      <c r="G6" s="17" t="n">
+      <c r="G6" s="16" t="n">
         <v>45000</v>
       </c>
-      <c r="H6" s="17" t="n">
+      <c r="H6" s="16" t="n">
         <v>54000</v>
       </c>
-      <c r="I6" s="17" t="n">
+      <c r="I6" s="16" t="n">
         <v>54000</v>
       </c>
-      <c r="J6" s="17" t="n">
+      <c r="J6" s="16" t="n">
         <v>54000</v>
       </c>
-      <c r="K6" s="17" t="n">
+      <c r="K6" s="16" t="n">
         <v>63000</v>
       </c>
-      <c r="L6" s="17" t="n">
+      <c r="L6" s="16" t="n">
         <v>63000</v>
       </c>
-      <c r="M6" s="17" t="n">
+      <c r="M6" s="16" t="n">
         <v>63000</v>
       </c>
-      <c r="N6" s="17" t="n">
+      <c r="N6" s="16" t="n">
         <v>65000</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="20" t="s">
+    <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="20" t="s">
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22" t="n">
+        <v>0.2098</v>
+      </c>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+    </row>
+    <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="14" t="s">
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22" t="n">
+        <v>0.23081</v>
+      </c>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+    </row>
+    <row r="9" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="23" t="n">
@@ -859,11 +856,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="14" t="s">
+    <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="23" t="n">
@@ -897,11 +894,11 @@
         <v>211000000000</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="14" t="s">
+    <row r="11" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="23" t="n">
@@ -935,43 +932,51 @@
         <v>7850</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="20" t="s">
+    <row r="12" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="20" t="s">
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="24" t="n">
+        <v>0.0239</v>
+      </c>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+    </row>
+    <row r="13" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-    </row>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="24" t="n">
+        <v>295310.34681</v>
+      </c>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>